<commit_message>
Preparing my first game.
</commit_message>
<xml_diff>
--- a/AssetsWorking/Data/Client/CharacterConfig.xlsx
+++ b/AssetsWorking/Data/Client/CharacterConfig.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>int</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -93,6 +93,26 @@
   </si>
   <si>
     <t>Assets/ExampleProject01/Res/Entities/Monster/10001/TargetPos.prefab</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>template</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>模板</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Character</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Character</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -488,23 +508,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13" style="1"/>
-    <col min="2" max="2" width="17.375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="39.875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="18.625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="63.25" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="13" style="1"/>
+    <col min="2" max="3" width="17.375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="39.875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18.625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="63.25" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="13" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -512,16 +532,19 @@
         <v>7</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -529,16 +552,19 @@
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -546,46 +572,55 @@
         <v>8</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="1">
-        <v>1</v>
+      <c r="C4" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="D4" s="1">
         <v>1</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="1">
         <v>2</v>
       </c>
-      <c r="D5" s="1">
+      <c r="E5" s="1">
         <v>1</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>